<commit_message>
update of tab documentation
</commit_message>
<xml_diff>
--- a/software_development/project/1 - Wires control with Potentiometer/UpdateFunction.xlsx
+++ b/software_development/project/1 - Wires control with Potentiometer/UpdateFunction.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\GitHub\BioticSystem\software_development\project\1 - Wires control with Potentiometer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8234442C-FABE-4A8D-98A7-1F0AEFE792B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623345A3-E6D1-4159-9EB7-3C2899FBEBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
   <si>
     <t>Statuts</t>
   </si>
@@ -237,9 +237,6 @@
     <t>WIRE3_OUT</t>
   </si>
   <si>
-    <t>Not Ready</t>
-  </si>
-  <si>
     <t>Display works</t>
   </si>
   <si>
@@ -313,6 +310,21 @@
   </si>
   <si>
     <t>Works with examples sketch of Arduino (use Servo.h lib)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC And Sensor works </t>
+  </si>
+  <si>
+    <t>Sensor works ! WARNING = not good precision</t>
+  </si>
+  <si>
+    <t>Works with the exemple</t>
+  </si>
+  <si>
+    <t>Test Ok</t>
+  </si>
+  <si>
+    <t>Execution problem with save fonctionality (in modification)</t>
   </si>
 </sst>
 </file>
@@ -929,47 +941,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -985,26 +968,14 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1012,9 +983,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1029,56 +997,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1086,14 +1012,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1104,71 +1024,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1177,38 +1054,170 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1226,16 +1235,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1517,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18:I20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,767 +1534,783 @@
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="45" t="s">
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="39" t="s">
+      <c r="J2" s="74"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="13"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="60"/>
     </row>
     <row r="3" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="L3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="33" t="s">
+      <c r="N3" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="20">
         <v>22</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="13">
         <v>45106</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="41" t="s">
+      <c r="L4" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="26">
+      <c r="M4" s="13">
         <v>45106</v>
       </c>
-      <c r="N4" s="27" t="s">
+      <c r="N4" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3" t="s">
+      <c r="B5" s="66"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="37">
+      <c r="H5" s="21">
         <v>24</v>
       </c>
-      <c r="I5" s="50"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="15"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="99">
+        <v>45112</v>
+      </c>
+      <c r="N5" s="100" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="53"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="55" t="s">
+      <c r="B6" s="67"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="55"/>
-      <c r="G6" s="56" t="s">
+      <c r="F6" s="26"/>
+      <c r="G6" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="57">
+      <c r="H6" s="27">
         <v>26</v>
       </c>
-      <c r="I6" s="58"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="63"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="31"/>
     </row>
     <row r="7" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="68" t="s">
+      <c r="E7" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="68" t="s">
+      <c r="F7" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="70" t="s">
+      <c r="I7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="71">
+      <c r="J7" s="38">
         <v>45106</v>
       </c>
-      <c r="K7" s="72" t="s">
+      <c r="K7" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="73" t="s">
+      <c r="L7" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="71">
+      <c r="M7" s="38">
         <v>45106</v>
       </c>
-      <c r="N7" s="72" t="s">
+      <c r="N7" s="39" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="49" t="s">
+      <c r="I8" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="13">
+        <v>45107</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="L8" s="79" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="13">
+        <v>45107</v>
+      </c>
+      <c r="N8" s="33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="66"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="77"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="67"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="78"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="29"/>
+    </row>
+    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="82" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="84" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="42"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="86" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="44">
+        <v>45106</v>
+      </c>
+      <c r="K11" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="64"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="M8" s="64"/>
-      <c r="N8" s="65"/>
-    </row>
-    <row r="9" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="37" t="s">
+      <c r="L11" s="88" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="44">
+        <v>45106</v>
+      </c>
+      <c r="N11" s="45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="66"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="66"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="66"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="66"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="66"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="83"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="87"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="20">
+        <v>46</v>
+      </c>
+      <c r="I18" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="32"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="M18" s="32"/>
+      <c r="N18" s="33"/>
+    </row>
+    <row r="19" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="66"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="21">
+        <v>45</v>
+      </c>
+      <c r="I19" s="77"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="80"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="6"/>
+    </row>
+    <row r="20" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="67"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="27">
+        <v>44</v>
+      </c>
+      <c r="I20" s="78"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="29"/>
+    </row>
+    <row r="21" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="82" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="84" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="84" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="43">
+        <v>43</v>
+      </c>
+      <c r="I21" s="90" t="s">
+        <v>98</v>
+      </c>
+      <c r="J21" s="44">
+        <v>45106</v>
+      </c>
+      <c r="K21" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="90" t="s">
+        <v>18</v>
+      </c>
+      <c r="M21" s="44">
+        <v>45106</v>
+      </c>
+      <c r="N21" s="45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="66"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="21">
         <v>42</v>
       </c>
-      <c r="I9" s="50"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="17"/>
-    </row>
-    <row r="10" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="56" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="56" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="58"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="60"/>
-    </row>
-    <row r="11" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="78" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="79" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="79" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="80" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="80" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="80"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="82" t="s">
+      <c r="I22" s="91"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="91"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="83"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="22">
+        <v>41</v>
+      </c>
+      <c r="I23" s="92"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="92"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="11"/>
+    </row>
+    <row r="24" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="96" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="93" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="93" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="43">
+        <v>5</v>
+      </c>
+      <c r="I24" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="83">
+      <c r="J24" s="44">
         <v>45106</v>
       </c>
-      <c r="K11" s="84" t="s">
-        <v>71</v>
-      </c>
-      <c r="L11" s="85" t="s">
+      <c r="K24" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="L24" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="83">
-        <v>45106</v>
-      </c>
-      <c r="N11" s="84" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="17"/>
-    </row>
-    <row r="13" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="17"/>
-    </row>
-    <row r="14" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="17"/>
-    </row>
-    <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="14"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="17"/>
-    </row>
-    <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="17"/>
-    </row>
-    <row r="17" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="86"/>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="88"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="89"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="22"/>
-    </row>
-    <row r="18" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="36">
-        <v>46</v>
-      </c>
-      <c r="I18" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="J18" s="64"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="M18" s="64"/>
-      <c r="N18" s="65"/>
-    </row>
-    <row r="19" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="37">
-        <v>45</v>
-      </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="17"/>
-    </row>
-    <row r="20" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="57">
-        <v>44</v>
-      </c>
-      <c r="I20" s="58"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="59"/>
-      <c r="N20" s="60"/>
-    </row>
-    <row r="21" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="78" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="90" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="90" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="80" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="80" t="s">
-        <v>77</v>
-      </c>
-      <c r="H21" s="81">
-        <v>43</v>
-      </c>
-      <c r="I21" s="103" t="s">
-        <v>70</v>
-      </c>
-      <c r="J21" s="83">
-        <v>45106</v>
-      </c>
-      <c r="K21" s="84" t="s">
-        <v>93</v>
-      </c>
-      <c r="L21" s="103" t="s">
-        <v>18</v>
-      </c>
-      <c r="M21" s="83">
-        <v>45106</v>
-      </c>
-      <c r="N21" s="84" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="14"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H22" s="37">
-        <v>42</v>
-      </c>
-      <c r="I22" s="104"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="17"/>
-    </row>
-    <row r="23" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="86"/>
-      <c r="C23" s="92"/>
-      <c r="D23" s="92"/>
-      <c r="E23" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="H23" s="38">
-        <v>41</v>
-      </c>
-      <c r="I23" s="105"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="105"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="22"/>
-    </row>
-    <row r="24" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="97" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="98" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="98" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="80" t="s">
+      <c r="M24" s="44">
+        <v>45107</v>
+      </c>
+      <c r="N24" s="45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="97"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="F24" s="80" t="s">
-        <v>89</v>
-      </c>
-      <c r="G24" s="80" t="s">
+      <c r="F25" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="H24" s="81">
-        <v>5</v>
-      </c>
-      <c r="I24" s="103" t="s">
-        <v>18</v>
-      </c>
-      <c r="J24" s="83">
-        <v>45106</v>
-      </c>
-      <c r="K24" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="L24" s="103" t="s">
-        <v>70</v>
-      </c>
-      <c r="M24" s="91"/>
-      <c r="N24" s="84"/>
-    </row>
-    <row r="25" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="99"/>
-      <c r="C25" s="100"/>
-      <c r="D25" s="100"/>
-      <c r="E25" s="25" t="s">
+      <c r="H25" s="20">
+        <v>6</v>
+      </c>
+      <c r="I25" s="91"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="91"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="33"/>
+    </row>
+    <row r="26" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="98"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F26" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="G26" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="36">
-        <v>6</v>
-      </c>
-      <c r="I25" s="104"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="104"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="65"/>
-    </row>
-    <row r="26" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="101"/>
-      <c r="C26" s="102"/>
-      <c r="D26" s="102"/>
-      <c r="E26" s="93" t="s">
-        <v>86</v>
-      </c>
-      <c r="F26" s="93" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26" s="93" t="s">
-        <v>92</v>
-      </c>
-      <c r="H26" s="94">
+      <c r="H26" s="47">
         <v>7</v>
       </c>
-      <c r="I26" s="105"/>
-      <c r="J26" s="95"/>
-      <c r="K26" s="96"/>
-      <c r="L26" s="105"/>
-      <c r="M26" s="95"/>
-      <c r="N26" s="96"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="92"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="49"/>
     </row>
     <row r="27" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="74"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="65"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="65"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="33"/>
     </row>
     <row r="28" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="74"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="77"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="65"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="54"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="33"/>
     </row>
     <row r="29" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="74"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="76"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="77"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="65"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="33"/>
     </row>
     <row r="30" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="74"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="77"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="65"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="33"/>
     </row>
     <row r="31" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="74"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="76"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="64"/>
-      <c r="N31" s="65"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="33"/>
     </row>
     <row r="32" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="16"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="37"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="21"/>
       <c r="I32" s="51"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="17"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="55"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="6"/>
     </row>
     <row r="33" spans="2:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="22"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="57"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="36">
@@ -2321,35 +2336,40 @@
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="B18:B20"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:K2"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="D4:D6"/>
     <mergeCell ref="I4:I6"/>
     <mergeCell ref="L4:L6"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
   </mergeCells>
-  <conditionalFormatting sqref="I4:I21 L4:L21 I24 I27:I33 L27:L33 L24">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="I4:I21 L4:L21 I24 L24 I27:I33 L27:L33">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Not Ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Ready"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I33 L4:L33">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Test ok"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 C7:C8 C11 C18 C21 C24 C27:C33" xr:uid="{DB3839FA-9E30-4A7B-A823-1CE56E1793D9}">
       <formula1>"Input, Output, In/Out"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11 L11 I18 I4:I8 I27:I33 L18 L4:L8 I21 I24 L27:L33 L21 L24" xr:uid="{60027EB8-A39C-4CC9-9414-1D24995B5335}">
-      <formula1>"Ready, Not Ready"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I33 L4:L33" xr:uid="{E9FE71BB-997F-4E54-868E-BCCBDA463F1F}">
+      <formula1>"Ready, Not Ready, Test Ok"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>